<commit_message>
First day for Mayu
</commit_message>
<xml_diff>
--- a/TFC_zaiko.xlsx
+++ b/TFC_zaiko.xlsx
@@ -563,7 +563,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,13 +571,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M323"/>
+  <dimension ref="A1:N326"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="H307" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J316" sqref="J316"/>
+      <selection pane="bottomRight" activeCell="N318" sqref="N318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -591,7 +591,7 @@
     <col min="14" max="1025" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,8 +606,9 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
@@ -622,8 +623,9 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -647,8 +649,9 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -662,8 +665,9 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -677,8 +681,9 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -692,8 +697,9 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -707,8 +713,9 @@
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -722,8 +729,9 @@
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -737,8 +745,9 @@
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N9" s="13"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -752,8 +761,9 @@
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N10" s="13"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -767,8 +777,9 @@
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -782,8 +793,9 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N12" s="13"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -797,8 +809,9 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -812,8 +825,9 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="13"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -827,8 +841,9 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="13"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -842,8 +857,9 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="13"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N16" s="13"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -857,8 +873,9 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="13"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -872,8 +889,9 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="13"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N18" s="13"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -887,8 +905,9 @@
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="13"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -902,8 +921,9 @@
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="13"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -917,8 +937,9 @@
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="M21" s="13"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N21" s="13"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -932,8 +953,9 @@
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="13"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -947,8 +969,9 @@
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="13"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -962,8 +985,9 @@
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
       <c r="M24" s="13"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -977,8 +1001,9 @@
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
       <c r="M25" s="13"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -992,8 +1017,9 @@
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
       <c r="M26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N26" s="13"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1007,8 +1033,9 @@
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="M27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N27" s="13"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1022,8 +1049,9 @@
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
       <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -1037,8 +1065,9 @@
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -1052,8 +1081,9 @@
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
       <c r="M30" s="13"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -1067,8 +1097,9 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="13"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -1082,8 +1113,9 @@
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="13"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N32" s="13"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -1097,8 +1129,9 @@
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
       <c r="M33" s="13"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -1112,8 +1145,9 @@
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
       <c r="M34" s="13"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -1127,8 +1161,9 @@
       <c r="K35" s="11"/>
       <c r="L35" s="11"/>
       <c r="M35" s="13"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -1142,8 +1177,9 @@
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="13"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N36" s="13"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -1157,8 +1193,9 @@
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
       <c r="M37" s="13"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N37" s="13"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -1172,8 +1209,9 @@
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
       <c r="M38" s="13"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N38" s="13"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -1187,8 +1225,9 @@
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
       <c r="M39" s="13"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N39" s="13"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -1202,8 +1241,9 @@
       <c r="K40" s="11"/>
       <c r="L40" s="11"/>
       <c r="M40" s="13"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N40" s="13"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -1217,8 +1257,9 @@
       <c r="K41" s="11"/>
       <c r="L41" s="11"/>
       <c r="M41" s="13"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -1232,8 +1273,9 @@
       <c r="K42" s="11"/>
       <c r="L42" s="11"/>
       <c r="M42" s="13"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N42" s="13"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -1247,8 +1289,9 @@
       <c r="K43" s="11"/>
       <c r="L43" s="11"/>
       <c r="M43" s="13"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N43" s="13"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -1262,8 +1305,9 @@
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
       <c r="M44" s="13"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N44" s="13"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -1277,8 +1321,9 @@
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
       <c r="M45" s="13"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N45" s="13"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -1292,8 +1337,9 @@
       <c r="K46" s="11"/>
       <c r="L46" s="11"/>
       <c r="M46" s="13"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -1307,8 +1353,9 @@
       <c r="K47" s="11"/>
       <c r="L47" s="11"/>
       <c r="M47" s="13"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N47" s="13"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -1322,8 +1369,9 @@
       <c r="K48" s="11"/>
       <c r="L48" s="11"/>
       <c r="M48" s="13"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N48" s="13"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -1337,8 +1385,9 @@
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
       <c r="M49" s="13"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N49" s="13"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -1352,8 +1401,9 @@
       <c r="K50" s="11"/>
       <c r="L50" s="11"/>
       <c r="M50" s="13"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N50" s="13"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -1367,8 +1417,9 @@
       <c r="K51" s="11"/>
       <c r="L51" s="11"/>
       <c r="M51" s="13"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N51" s="13"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -1382,8 +1433,9 @@
       <c r="K52" s="11"/>
       <c r="L52" s="11"/>
       <c r="M52" s="13"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N52" s="13"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -1397,8 +1449,9 @@
       <c r="K53" s="11"/>
       <c r="L53" s="11"/>
       <c r="M53" s="13"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N53" s="13"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -1412,8 +1465,9 @@
       <c r="K54" s="11"/>
       <c r="L54" s="11"/>
       <c r="M54" s="13"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N54" s="13"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A55" s="11"/>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
@@ -1427,8 +1481,9 @@
       <c r="K55" s="11"/>
       <c r="L55" s="11"/>
       <c r="M55" s="13"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N55" s="13"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A56" s="11"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -1442,8 +1497,9 @@
       <c r="K56" s="11"/>
       <c r="L56" s="11"/>
       <c r="M56" s="13"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N56" s="13"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A57" s="11"/>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
@@ -1457,8 +1513,9 @@
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
       <c r="M57" s="13"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N57" s="13"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -1472,8 +1529,9 @@
       <c r="K58" s="11"/>
       <c r="L58" s="11"/>
       <c r="M58" s="13"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N58" s="13"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -1487,8 +1545,9 @@
       <c r="K59" s="11"/>
       <c r="L59" s="11"/>
       <c r="M59" s="13"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N59" s="13"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A60" s="11"/>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -1502,8 +1561,9 @@
       <c r="K60" s="11"/>
       <c r="L60" s="11"/>
       <c r="M60" s="13"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N60" s="13"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A61" s="11"/>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
@@ -1517,8 +1577,9 @@
       <c r="K61" s="11"/>
       <c r="L61" s="11"/>
       <c r="M61" s="13"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N61" s="13"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -1532,8 +1593,9 @@
       <c r="K62" s="11"/>
       <c r="L62" s="11"/>
       <c r="M62" s="13"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N62" s="13"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -1547,8 +1609,9 @@
       <c r="K63" s="11"/>
       <c r="L63" s="11"/>
       <c r="M63" s="13"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N63" s="13"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -1562,8 +1625,9 @@
       <c r="K64" s="11"/>
       <c r="L64" s="11"/>
       <c r="M64" s="13"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N64" s="13"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A65" s="11"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -1577,8 +1641,9 @@
       <c r="K65" s="11"/>
       <c r="L65" s="11"/>
       <c r="M65" s="13"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A66" s="11"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -1592,8 +1657,9 @@
       <c r="K66" s="11"/>
       <c r="L66" s="11"/>
       <c r="M66" s="13"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N66" s="13"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -1607,8 +1673,9 @@
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
       <c r="M67" s="13"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N67" s="13"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
@@ -1622,8 +1689,9 @@
       <c r="K68" s="11"/>
       <c r="L68" s="11"/>
       <c r="M68" s="13"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N68" s="13"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A69" s="11"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -1637,8 +1705,9 @@
       <c r="K69" s="11"/>
       <c r="L69" s="11"/>
       <c r="M69" s="13"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N69" s="13"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A70" s="11"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -1652,8 +1721,9 @@
       <c r="K70" s="11"/>
       <c r="L70" s="11"/>
       <c r="M70" s="13"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N70" s="13"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
@@ -1667,8 +1737,9 @@
       <c r="K71" s="11"/>
       <c r="L71" s="11"/>
       <c r="M71" s="13"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N71" s="13"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A72" s="11"/>
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
@@ -1682,8 +1753,9 @@
       <c r="K72" s="11"/>
       <c r="L72" s="11"/>
       <c r="M72" s="13"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N72" s="13"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A73" s="11"/>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
@@ -1697,8 +1769,9 @@
       <c r="K73" s="11"/>
       <c r="L73" s="11"/>
       <c r="M73" s="13"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N73" s="13"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A74" s="11"/>
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
@@ -1712,8 +1785,9 @@
       <c r="K74" s="11"/>
       <c r="L74" s="11"/>
       <c r="M74" s="13"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N74" s="13"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A75" s="11"/>
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
@@ -1727,8 +1801,9 @@
       <c r="K75" s="11"/>
       <c r="L75" s="11"/>
       <c r="M75" s="13"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N75" s="13"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A76" s="11"/>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -1742,8 +1817,9 @@
       <c r="K76" s="11"/>
       <c r="L76" s="11"/>
       <c r="M76" s="13"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N76" s="13"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -1757,8 +1833,9 @@
       <c r="K77" s="11"/>
       <c r="L77" s="11"/>
       <c r="M77" s="13"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N77" s="13"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
@@ -1772,8 +1849,9 @@
       <c r="K78" s="11"/>
       <c r="L78" s="11"/>
       <c r="M78" s="13"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N78" s="13"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -1787,8 +1865,9 @@
       <c r="K79" s="11"/>
       <c r="L79" s="11"/>
       <c r="M79" s="13"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N79" s="13"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A80" s="11"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -1802,8 +1881,9 @@
       <c r="K80" s="11"/>
       <c r="L80" s="11"/>
       <c r="M80" s="13"/>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N80" s="13"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A81" s="11"/>
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
@@ -1817,8 +1897,9 @@
       <c r="K81" s="11"/>
       <c r="L81" s="11"/>
       <c r="M81" s="13"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N81" s="13"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
@@ -1832,8 +1913,9 @@
       <c r="K82" s="11"/>
       <c r="L82" s="11"/>
       <c r="M82" s="13"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N82" s="13"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
@@ -1847,8 +1929,9 @@
       <c r="K83" s="11"/>
       <c r="L83" s="11"/>
       <c r="M83" s="13"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N83" s="13"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A84" s="11"/>
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
@@ -1862,8 +1945,9 @@
       <c r="K84" s="11"/>
       <c r="L84" s="11"/>
       <c r="M84" s="13"/>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N84" s="13"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A85" s="11"/>
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
@@ -1877,8 +1961,9 @@
       <c r="K85" s="11"/>
       <c r="L85" s="11"/>
       <c r="M85" s="13"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N85" s="13"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
@@ -1892,8 +1977,9 @@
       <c r="K86" s="11"/>
       <c r="L86" s="11"/>
       <c r="M86" s="13"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N86" s="13"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A87" s="11"/>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
@@ -1907,8 +1993,9 @@
       <c r="K87" s="11"/>
       <c r="L87" s="11"/>
       <c r="M87" s="13"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N87" s="13"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
@@ -1922,8 +2009,9 @@
       <c r="K88" s="11"/>
       <c r="L88" s="11"/>
       <c r="M88" s="13"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N88" s="13"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A89" s="11"/>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
@@ -1937,8 +2025,9 @@
       <c r="K89" s="11"/>
       <c r="L89" s="11"/>
       <c r="M89" s="13"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N89" s="13"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A90" s="11"/>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
@@ -1952,8 +2041,9 @@
       <c r="K90" s="11"/>
       <c r="L90" s="11"/>
       <c r="M90" s="13"/>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N90" s="13"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A91" s="11"/>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
@@ -1967,8 +2057,9 @@
       <c r="K91" s="11"/>
       <c r="L91" s="11"/>
       <c r="M91" s="13"/>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N91" s="13"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A92" s="11"/>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -1982,8 +2073,9 @@
       <c r="K92" s="11"/>
       <c r="L92" s="11"/>
       <c r="M92" s="13"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N92" s="13"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A93" s="11"/>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -1997,8 +2089,9 @@
       <c r="K93" s="11"/>
       <c r="L93" s="11"/>
       <c r="M93" s="13"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N93" s="13"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A94" s="11"/>
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
@@ -2012,8 +2105,9 @@
       <c r="K94" s="11"/>
       <c r="L94" s="11"/>
       <c r="M94" s="13"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N94" s="13"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A95" s="11"/>
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>
@@ -2027,8 +2121,9 @@
       <c r="K95" s="11"/>
       <c r="L95" s="11"/>
       <c r="M95" s="13"/>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N95" s="13"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A96" s="11"/>
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
@@ -2042,8 +2137,9 @@
       <c r="K96" s="11"/>
       <c r="L96" s="11"/>
       <c r="M96" s="13"/>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N96" s="13"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A97" s="11"/>
       <c r="B97" s="11"/>
       <c r="C97" s="11"/>
@@ -2057,8 +2153,9 @@
       <c r="K97" s="11"/>
       <c r="L97" s="11"/>
       <c r="M97" s="13"/>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N97" s="13"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A98" s="11"/>
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
@@ -2072,8 +2169,9 @@
       <c r="K98" s="11"/>
       <c r="L98" s="11"/>
       <c r="M98" s="13"/>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N98" s="13"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A99" s="11"/>
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
@@ -2087,8 +2185,9 @@
       <c r="K99" s="11"/>
       <c r="L99" s="11"/>
       <c r="M99" s="13"/>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N99" s="13"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A100" s="11"/>
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
@@ -2102,8 +2201,9 @@
       <c r="K100" s="11"/>
       <c r="L100" s="11"/>
       <c r="M100" s="13"/>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N100" s="13"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A101" s="11"/>
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
@@ -2117,8 +2217,9 @@
       <c r="K101" s="11"/>
       <c r="L101" s="11"/>
       <c r="M101" s="13"/>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N101" s="13"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A102" s="11"/>
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
@@ -2132,8 +2233,9 @@
       <c r="K102" s="11"/>
       <c r="L102" s="11"/>
       <c r="M102" s="13"/>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N102" s="13"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A103" s="11"/>
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
@@ -2147,8 +2249,9 @@
       <c r="K103" s="11"/>
       <c r="L103" s="11"/>
       <c r="M103" s="13"/>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N103" s="13"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A104" s="11"/>
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
@@ -2162,8 +2265,9 @@
       <c r="K104" s="11"/>
       <c r="L104" s="11"/>
       <c r="M104" s="13"/>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N104" s="13"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A105" s="11"/>
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
@@ -2177,8 +2281,9 @@
       <c r="K105" s="11"/>
       <c r="L105" s="11"/>
       <c r="M105" s="13"/>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N105" s="13"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A106" s="11"/>
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
@@ -2192,8 +2297,9 @@
       <c r="K106" s="11"/>
       <c r="L106" s="11"/>
       <c r="M106" s="13"/>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N106" s="13"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A107" s="11"/>
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
@@ -2207,8 +2313,9 @@
       <c r="K107" s="11"/>
       <c r="L107" s="11"/>
       <c r="M107" s="13"/>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N107" s="13"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A108" s="11"/>
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
@@ -2222,8 +2329,9 @@
       <c r="K108" s="11"/>
       <c r="L108" s="11"/>
       <c r="M108" s="13"/>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N108" s="13"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A109" s="11"/>
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
@@ -2237,8 +2345,9 @@
       <c r="K109" s="11"/>
       <c r="L109" s="11"/>
       <c r="M109" s="13"/>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N109" s="13"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A110" s="11"/>
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
@@ -2252,8 +2361,9 @@
       <c r="K110" s="11"/>
       <c r="L110" s="11"/>
       <c r="M110" s="13"/>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N110" s="13"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A111" s="11"/>
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
@@ -2267,8 +2377,9 @@
       <c r="K111" s="11"/>
       <c r="L111" s="11"/>
       <c r="M111" s="13"/>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N111" s="13"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A112" s="11"/>
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
@@ -2282,8 +2393,9 @@
       <c r="K112" s="11"/>
       <c r="L112" s="11"/>
       <c r="M112" s="13"/>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N112" s="13"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A113" s="11"/>
       <c r="B113" s="11"/>
       <c r="C113" s="11"/>
@@ -2297,8 +2409,9 @@
       <c r="K113" s="11"/>
       <c r="L113" s="11"/>
       <c r="M113" s="13"/>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N113" s="13"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A114" s="11"/>
       <c r="B114" s="11"/>
       <c r="C114" s="11"/>
@@ -2312,8 +2425,9 @@
       <c r="K114" s="11"/>
       <c r="L114" s="11"/>
       <c r="M114" s="13"/>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N114" s="13"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A115" s="11"/>
       <c r="B115" s="11"/>
       <c r="C115" s="11"/>
@@ -2327,8 +2441,9 @@
       <c r="K115" s="11"/>
       <c r="L115" s="11"/>
       <c r="M115" s="13"/>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N115" s="13"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A116" s="11"/>
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
@@ -2342,8 +2457,9 @@
       <c r="K116" s="11"/>
       <c r="L116" s="11"/>
       <c r="M116" s="13"/>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N116" s="13"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A117" s="11"/>
       <c r="B117" s="11"/>
       <c r="C117" s="11"/>
@@ -2357,8 +2473,9 @@
       <c r="K117" s="11"/>
       <c r="L117" s="11"/>
       <c r="M117" s="13"/>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N117" s="13"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A118" s="11"/>
       <c r="B118" s="11"/>
       <c r="C118" s="11"/>
@@ -2372,8 +2489,9 @@
       <c r="K118" s="11"/>
       <c r="L118" s="11"/>
       <c r="M118" s="13"/>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N118" s="13"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A119" s="11"/>
       <c r="B119" s="11"/>
       <c r="C119" s="11"/>
@@ -2387,8 +2505,9 @@
       <c r="K119" s="11"/>
       <c r="L119" s="11"/>
       <c r="M119" s="13"/>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N119" s="13"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A120" s="11"/>
       <c r="B120" s="11"/>
       <c r="C120" s="11"/>
@@ -2402,8 +2521,9 @@
       <c r="K120" s="11"/>
       <c r="L120" s="11"/>
       <c r="M120" s="13"/>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N120" s="13"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A121" s="11"/>
       <c r="B121" s="11"/>
       <c r="C121" s="11"/>
@@ -2417,8 +2537,9 @@
       <c r="K121" s="11"/>
       <c r="L121" s="11"/>
       <c r="M121" s="13"/>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N121" s="13"/>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A122" s="11"/>
       <c r="B122" s="11"/>
       <c r="C122" s="11"/>
@@ -2432,8 +2553,9 @@
       <c r="K122" s="11"/>
       <c r="L122" s="11"/>
       <c r="M122" s="13"/>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N122" s="13"/>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A123" s="11"/>
       <c r="B123" s="11"/>
       <c r="C123" s="11"/>
@@ -2447,8 +2569,9 @@
       <c r="K123" s="11"/>
       <c r="L123" s="11"/>
       <c r="M123" s="13"/>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N123" s="13"/>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A124" s="11"/>
       <c r="B124" s="11"/>
       <c r="C124" s="11"/>
@@ -2462,8 +2585,9 @@
       <c r="K124" s="11"/>
       <c r="L124" s="11"/>
       <c r="M124" s="13"/>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N124" s="13"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A125" s="11"/>
       <c r="B125" s="11"/>
       <c r="C125" s="11"/>
@@ -2477,8 +2601,9 @@
       <c r="K125" s="11"/>
       <c r="L125" s="11"/>
       <c r="M125" s="13"/>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N125" s="13"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A126" s="11"/>
       <c r="B126" s="11"/>
       <c r="C126" s="11"/>
@@ -2492,8 +2617,9 @@
       <c r="K126" s="11"/>
       <c r="L126" s="11"/>
       <c r="M126" s="13"/>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N126" s="13"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A127" s="11"/>
       <c r="B127" s="11"/>
       <c r="C127" s="11"/>
@@ -2507,8 +2633,9 @@
       <c r="K127" s="11"/>
       <c r="L127" s="11"/>
       <c r="M127" s="13"/>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N127" s="13"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A128" s="11"/>
       <c r="B128" s="11"/>
       <c r="C128" s="11"/>
@@ -2522,8 +2649,9 @@
       <c r="K128" s="11"/>
       <c r="L128" s="11"/>
       <c r="M128" s="13"/>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N128" s="13"/>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A129" s="11"/>
       <c r="B129" s="11"/>
       <c r="C129" s="11"/>
@@ -2537,8 +2665,9 @@
       <c r="K129" s="11"/>
       <c r="L129" s="11"/>
       <c r="M129" s="13"/>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N129" s="13"/>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A130" s="11"/>
       <c r="B130" s="11"/>
       <c r="C130" s="11"/>
@@ -2552,8 +2681,9 @@
       <c r="K130" s="11"/>
       <c r="L130" s="11"/>
       <c r="M130" s="13"/>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N130" s="13"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A131" s="11"/>
       <c r="B131" s="11"/>
       <c r="C131" s="11"/>
@@ -2567,8 +2697,9 @@
       <c r="K131" s="11"/>
       <c r="L131" s="11"/>
       <c r="M131" s="13"/>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N131" s="13"/>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A132" s="11"/>
       <c r="B132" s="11"/>
       <c r="C132" s="11"/>
@@ -2582,8 +2713,9 @@
       <c r="K132" s="11"/>
       <c r="L132" s="11"/>
       <c r="M132" s="13"/>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N132" s="13"/>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A133" s="11"/>
       <c r="B133" s="11"/>
       <c r="C133" s="11"/>
@@ -2597,8 +2729,9 @@
       <c r="K133" s="11"/>
       <c r="L133" s="11"/>
       <c r="M133" s="13"/>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N133" s="13"/>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A134" s="11"/>
       <c r="B134" s="11"/>
       <c r="C134" s="11"/>
@@ -2612,8 +2745,9 @@
       <c r="K134" s="11"/>
       <c r="L134" s="11"/>
       <c r="M134" s="13"/>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N134" s="13"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A135" s="11"/>
       <c r="B135" s="11"/>
       <c r="C135" s="11"/>
@@ -2627,8 +2761,9 @@
       <c r="K135" s="11"/>
       <c r="L135" s="11"/>
       <c r="M135" s="13"/>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N135" s="13"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A136" s="11"/>
       <c r="B136" s="11"/>
       <c r="C136" s="11"/>
@@ -2642,8 +2777,9 @@
       <c r="K136" s="11"/>
       <c r="L136" s="11"/>
       <c r="M136" s="13"/>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N136" s="13"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A137" s="11"/>
       <c r="B137" s="11"/>
       <c r="C137" s="11"/>
@@ -2657,8 +2793,9 @@
       <c r="K137" s="11"/>
       <c r="L137" s="11"/>
       <c r="M137" s="13"/>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N137" s="13"/>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A138" s="11"/>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
@@ -2672,8 +2809,9 @@
       <c r="K138" s="11"/>
       <c r="L138" s="11"/>
       <c r="M138" s="13"/>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N138" s="13"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A139" s="11"/>
       <c r="B139" s="11"/>
       <c r="C139" s="11"/>
@@ -2687,8 +2825,9 @@
       <c r="K139" s="11"/>
       <c r="L139" s="11"/>
       <c r="M139" s="13"/>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N139" s="13"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A140" s="11"/>
       <c r="B140" s="11"/>
       <c r="C140" s="11"/>
@@ -2702,8 +2841,9 @@
       <c r="K140" s="11"/>
       <c r="L140" s="11"/>
       <c r="M140" s="13"/>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N140" s="13"/>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A141" s="11"/>
       <c r="B141" s="11"/>
       <c r="C141" s="11"/>
@@ -2717,8 +2857,9 @@
       <c r="K141" s="11"/>
       <c r="L141" s="11"/>
       <c r="M141" s="13"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N141" s="13"/>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A142" s="11"/>
       <c r="B142" s="11"/>
       <c r="C142" s="11"/>
@@ -2732,8 +2873,9 @@
       <c r="K142" s="11"/>
       <c r="L142" s="11"/>
       <c r="M142" s="13"/>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N142" s="13"/>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A143" s="11"/>
       <c r="B143" s="11"/>
       <c r="C143" s="11"/>
@@ -2747,8 +2889,9 @@
       <c r="K143" s="11"/>
       <c r="L143" s="11"/>
       <c r="M143" s="13"/>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N143" s="13"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A144" s="11"/>
       <c r="B144" s="11"/>
       <c r="C144" s="11"/>
@@ -2762,8 +2905,9 @@
       <c r="K144" s="11"/>
       <c r="L144" s="11"/>
       <c r="M144" s="13"/>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N144" s="13"/>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A145" s="11"/>
       <c r="B145" s="11"/>
       <c r="C145" s="11"/>
@@ -2777,8 +2921,9 @@
       <c r="K145" s="11"/>
       <c r="L145" s="11"/>
       <c r="M145" s="13"/>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N145" s="13"/>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A146" s="11"/>
       <c r="B146" s="11"/>
       <c r="C146" s="11"/>
@@ -2792,8 +2937,9 @@
       <c r="K146" s="11"/>
       <c r="L146" s="11"/>
       <c r="M146" s="13"/>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N146" s="13"/>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A147" s="11"/>
       <c r="B147" s="11"/>
       <c r="C147" s="11"/>
@@ -2807,8 +2953,9 @@
       <c r="K147" s="11"/>
       <c r="L147" s="11"/>
       <c r="M147" s="13"/>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N147" s="13"/>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A148" s="11"/>
       <c r="B148" s="11"/>
       <c r="C148" s="11"/>
@@ -2822,8 +2969,9 @@
       <c r="K148" s="11"/>
       <c r="L148" s="11"/>
       <c r="M148" s="13"/>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N148" s="13"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A149" s="11"/>
       <c r="B149" s="11"/>
       <c r="C149" s="11"/>
@@ -2837,8 +2985,9 @@
       <c r="K149" s="11"/>
       <c r="L149" s="11"/>
       <c r="M149" s="13"/>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N149" s="13"/>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A150" s="11"/>
       <c r="B150" s="11"/>
       <c r="C150" s="11"/>
@@ -2852,8 +3001,9 @@
       <c r="K150" s="11"/>
       <c r="L150" s="11"/>
       <c r="M150" s="13"/>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N150" s="13"/>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A151" s="11"/>
       <c r="B151" s="11"/>
       <c r="C151" s="11"/>
@@ -2867,8 +3017,9 @@
       <c r="K151" s="11"/>
       <c r="L151" s="11"/>
       <c r="M151" s="13"/>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N151" s="13"/>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A152" s="11"/>
       <c r="B152" s="11"/>
       <c r="C152" s="11"/>
@@ -2882,8 +3033,9 @@
       <c r="K152" s="11"/>
       <c r="L152" s="11"/>
       <c r="M152" s="13"/>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N152" s="13"/>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A153" s="11"/>
       <c r="B153" s="11"/>
       <c r="C153" s="11"/>
@@ -2897,8 +3049,9 @@
       <c r="K153" s="11"/>
       <c r="L153" s="11"/>
       <c r="M153" s="13"/>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N153" s="13"/>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A154" s="11"/>
       <c r="B154" s="11"/>
       <c r="C154" s="11"/>
@@ -2912,8 +3065,9 @@
       <c r="K154" s="11"/>
       <c r="L154" s="11"/>
       <c r="M154" s="13"/>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N154" s="13"/>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A155" s="11"/>
       <c r="B155" s="11"/>
       <c r="C155" s="11"/>
@@ -2927,8 +3081,9 @@
       <c r="K155" s="11"/>
       <c r="L155" s="11"/>
       <c r="M155" s="13"/>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N155" s="13"/>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A156" s="11"/>
       <c r="B156" s="11"/>
       <c r="C156" s="11"/>
@@ -2942,8 +3097,9 @@
       <c r="K156" s="11"/>
       <c r="L156" s="11"/>
       <c r="M156" s="13"/>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N156" s="13"/>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A157" s="11"/>
       <c r="B157" s="11"/>
       <c r="C157" s="11"/>
@@ -2957,8 +3113,9 @@
       <c r="K157" s="11"/>
       <c r="L157" s="11"/>
       <c r="M157" s="13"/>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N157" s="13"/>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A158" s="11"/>
       <c r="B158" s="11"/>
       <c r="C158" s="11"/>
@@ -2972,8 +3129,9 @@
       <c r="K158" s="11"/>
       <c r="L158" s="11"/>
       <c r="M158" s="13"/>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N158" s="13"/>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A159" s="11"/>
       <c r="B159" s="11"/>
       <c r="C159" s="11"/>
@@ -2987,8 +3145,9 @@
       <c r="K159" s="11"/>
       <c r="L159" s="11"/>
       <c r="M159" s="13"/>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N159" s="13"/>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A160" s="11"/>
       <c r="B160" s="11"/>
       <c r="C160" s="11"/>
@@ -3002,8 +3161,9 @@
       <c r="K160" s="11"/>
       <c r="L160" s="11"/>
       <c r="M160" s="13"/>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N160" s="13"/>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A161" s="11"/>
       <c r="B161" s="11"/>
       <c r="C161" s="11"/>
@@ -3017,8 +3177,9 @@
       <c r="K161" s="11"/>
       <c r="L161" s="11"/>
       <c r="M161" s="13"/>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N161" s="13"/>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A162" s="11"/>
       <c r="B162" s="11"/>
       <c r="C162" s="11"/>
@@ -3032,8 +3193,9 @@
       <c r="K162" s="11"/>
       <c r="L162" s="11"/>
       <c r="M162" s="13"/>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N162" s="13"/>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A163" s="11"/>
       <c r="B163" s="11"/>
       <c r="C163" s="11"/>
@@ -3047,8 +3209,9 @@
       <c r="K163" s="11"/>
       <c r="L163" s="11"/>
       <c r="M163" s="13"/>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N163" s="13"/>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A164" s="11"/>
       <c r="B164" s="11"/>
       <c r="C164" s="11"/>
@@ -3062,8 +3225,9 @@
       <c r="K164" s="11"/>
       <c r="L164" s="11"/>
       <c r="M164" s="13"/>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N164" s="13"/>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A165" s="11"/>
       <c r="B165" s="11"/>
       <c r="C165" s="11"/>
@@ -3077,8 +3241,9 @@
       <c r="K165" s="11"/>
       <c r="L165" s="11"/>
       <c r="M165" s="13"/>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N165" s="13"/>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A166" s="11"/>
       <c r="B166" s="11"/>
       <c r="C166" s="11"/>
@@ -3092,8 +3257,9 @@
       <c r="K166" s="11"/>
       <c r="L166" s="11"/>
       <c r="M166" s="13"/>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N166" s="13"/>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A167" s="11"/>
       <c r="B167" s="11"/>
       <c r="C167" s="11"/>
@@ -3107,8 +3273,9 @@
       <c r="K167" s="11"/>
       <c r="L167" s="11"/>
       <c r="M167" s="13"/>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N167" s="13"/>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A168" s="11"/>
       <c r="B168" s="11"/>
       <c r="C168" s="11"/>
@@ -3122,8 +3289,9 @@
       <c r="K168" s="11"/>
       <c r="L168" s="11"/>
       <c r="M168" s="13"/>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N168" s="13"/>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A169" s="11"/>
       <c r="B169" s="11"/>
       <c r="C169" s="11"/>
@@ -3137,8 +3305,9 @@
       <c r="K169" s="11"/>
       <c r="L169" s="11"/>
       <c r="M169" s="13"/>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N169" s="13"/>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A170" s="11"/>
       <c r="B170" s="11"/>
       <c r="C170" s="11"/>
@@ -3152,8 +3321,9 @@
       <c r="K170" s="11"/>
       <c r="L170" s="11"/>
       <c r="M170" s="13"/>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N170" s="13"/>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A171" s="11"/>
       <c r="B171" s="11"/>
       <c r="C171" s="11"/>
@@ -3167,8 +3337,9 @@
       <c r="K171" s="11"/>
       <c r="L171" s="11"/>
       <c r="M171" s="13"/>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N171" s="13"/>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A172" s="11"/>
       <c r="B172" s="11"/>
       <c r="C172" s="11"/>
@@ -3182,8 +3353,9 @@
       <c r="K172" s="11"/>
       <c r="L172" s="11"/>
       <c r="M172" s="13"/>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N172" s="13"/>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A173" s="11"/>
       <c r="B173" s="11"/>
       <c r="C173" s="11"/>
@@ -3197,8 +3369,9 @@
       <c r="K173" s="11"/>
       <c r="L173" s="11"/>
       <c r="M173" s="13"/>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N173" s="13"/>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A174" s="11"/>
       <c r="B174" s="11"/>
       <c r="C174" s="11"/>
@@ -3212,8 +3385,9 @@
       <c r="K174" s="11"/>
       <c r="L174" s="11"/>
       <c r="M174" s="13"/>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N174" s="13"/>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A175" s="11"/>
       <c r="B175" s="11"/>
       <c r="C175" s="11"/>
@@ -3227,8 +3401,9 @@
       <c r="K175" s="11"/>
       <c r="L175" s="11"/>
       <c r="M175" s="13"/>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N175" s="13"/>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A176" s="11"/>
       <c r="B176" s="11"/>
       <c r="C176" s="11"/>
@@ -3242,8 +3417,9 @@
       <c r="K176" s="11"/>
       <c r="L176" s="11"/>
       <c r="M176" s="13"/>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N176" s="13"/>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A177" s="11"/>
       <c r="B177" s="11"/>
       <c r="C177" s="11"/>
@@ -3257,8 +3433,9 @@
       <c r="K177" s="11"/>
       <c r="L177" s="11"/>
       <c r="M177" s="13"/>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N177" s="13"/>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A178" s="11"/>
       <c r="B178" s="11"/>
       <c r="C178" s="11"/>
@@ -3272,8 +3449,9 @@
       <c r="K178" s="11"/>
       <c r="L178" s="11"/>
       <c r="M178" s="13"/>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N178" s="13"/>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A179" s="11"/>
       <c r="B179" s="11"/>
       <c r="C179" s="11"/>
@@ -3287,8 +3465,9 @@
       <c r="K179" s="11"/>
       <c r="L179" s="11"/>
       <c r="M179" s="13"/>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N179" s="13"/>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A180" s="11"/>
       <c r="B180" s="11"/>
       <c r="C180" s="11"/>
@@ -3302,8 +3481,9 @@
       <c r="K180" s="11"/>
       <c r="L180" s="11"/>
       <c r="M180" s="13"/>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N180" s="13"/>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A181" s="11"/>
       <c r="B181" s="11"/>
       <c r="C181" s="11"/>
@@ -3317,8 +3497,9 @@
       <c r="K181" s="11"/>
       <c r="L181" s="11"/>
       <c r="M181" s="13"/>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N181" s="13"/>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A182" s="11"/>
       <c r="B182" s="11"/>
       <c r="C182" s="11"/>
@@ -3332,8 +3513,9 @@
       <c r="K182" s="11"/>
       <c r="L182" s="11"/>
       <c r="M182" s="13"/>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N182" s="13"/>
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A183" s="11"/>
       <c r="B183" s="11"/>
       <c r="C183" s="11"/>
@@ -3347,8 +3529,9 @@
       <c r="K183" s="11"/>
       <c r="L183" s="11"/>
       <c r="M183" s="13"/>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N183" s="13"/>
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A184" s="11"/>
       <c r="B184" s="11"/>
       <c r="C184" s="11"/>
@@ -3362,8 +3545,9 @@
       <c r="K184" s="11"/>
       <c r="L184" s="11"/>
       <c r="M184" s="13"/>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N184" s="13"/>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A185" s="11"/>
       <c r="B185" s="11"/>
       <c r="C185" s="11"/>
@@ -3377,8 +3561,9 @@
       <c r="K185" s="11"/>
       <c r="L185" s="11"/>
       <c r="M185" s="13"/>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N185" s="13"/>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A186" s="11"/>
       <c r="B186" s="11"/>
       <c r="C186" s="11"/>
@@ -3392,8 +3577,9 @@
       <c r="K186" s="11"/>
       <c r="L186" s="11"/>
       <c r="M186" s="13"/>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N186" s="13"/>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A187" s="11"/>
       <c r="B187" s="11"/>
       <c r="C187" s="11"/>
@@ -3407,8 +3593,9 @@
       <c r="K187" s="11"/>
       <c r="L187" s="11"/>
       <c r="M187" s="13"/>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N187" s="13"/>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A188" s="11"/>
       <c r="B188" s="11"/>
       <c r="C188" s="11"/>
@@ -3422,8 +3609,9 @@
       <c r="K188" s="11"/>
       <c r="L188" s="11"/>
       <c r="M188" s="13"/>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N188" s="13"/>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A189" s="11"/>
       <c r="B189" s="11"/>
       <c r="C189" s="11"/>
@@ -3437,8 +3625,9 @@
       <c r="K189" s="11"/>
       <c r="L189" s="11"/>
       <c r="M189" s="13"/>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N189" s="13"/>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A190" s="11"/>
       <c r="B190" s="11"/>
       <c r="C190" s="11"/>
@@ -3452,8 +3641,9 @@
       <c r="K190" s="11"/>
       <c r="L190" s="11"/>
       <c r="M190" s="13"/>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N190" s="13"/>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A191" s="11"/>
       <c r="B191" s="11"/>
       <c r="C191" s="11"/>
@@ -3467,8 +3657,9 @@
       <c r="K191" s="11"/>
       <c r="L191" s="11"/>
       <c r="M191" s="13"/>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N191" s="13"/>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A192" s="11"/>
       <c r="B192" s="11"/>
       <c r="C192" s="11"/>
@@ -3482,8 +3673,9 @@
       <c r="K192" s="11"/>
       <c r="L192" s="11"/>
       <c r="M192" s="13"/>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N192" s="13"/>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A193" s="11"/>
       <c r="B193" s="11"/>
       <c r="C193" s="11"/>
@@ -3497,8 +3689,9 @@
       <c r="K193" s="11"/>
       <c r="L193" s="11"/>
       <c r="M193" s="13"/>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N193" s="13"/>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A194" s="11"/>
       <c r="B194" s="11"/>
       <c r="C194" s="11"/>
@@ -3512,8 +3705,9 @@
       <c r="K194" s="11"/>
       <c r="L194" s="11"/>
       <c r="M194" s="13"/>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N194" s="13"/>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A195" s="11"/>
       <c r="B195" s="11"/>
       <c r="C195" s="11"/>
@@ -3527,8 +3721,9 @@
       <c r="K195" s="11"/>
       <c r="L195" s="11"/>
       <c r="M195" s="13"/>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N195" s="13"/>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A196" s="11"/>
       <c r="B196" s="11"/>
       <c r="C196" s="11"/>
@@ -3542,8 +3737,9 @@
       <c r="K196" s="11"/>
       <c r="L196" s="11"/>
       <c r="M196" s="13"/>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N196" s="13"/>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A197" s="11"/>
       <c r="B197" s="11"/>
       <c r="C197" s="11"/>
@@ -3557,8 +3753,9 @@
       <c r="K197" s="11"/>
       <c r="L197" s="11"/>
       <c r="M197" s="13"/>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N197" s="13"/>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A198" s="11"/>
       <c r="B198" s="11"/>
       <c r="C198" s="11"/>
@@ -3572,8 +3769,9 @@
       <c r="K198" s="11"/>
       <c r="L198" s="11"/>
       <c r="M198" s="13"/>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N198" s="13"/>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A199" s="11"/>
       <c r="B199" s="11"/>
       <c r="C199" s="11"/>
@@ -3587,8 +3785,9 @@
       <c r="K199" s="11"/>
       <c r="L199" s="11"/>
       <c r="M199" s="13"/>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N199" s="13"/>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A200" s="11"/>
       <c r="B200" s="11"/>
       <c r="C200" s="11"/>
@@ -3602,8 +3801,9 @@
       <c r="K200" s="11"/>
       <c r="L200" s="11"/>
       <c r="M200" s="13"/>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N200" s="13"/>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A201" s="11"/>
       <c r="B201" s="11"/>
       <c r="C201" s="11"/>
@@ -3617,8 +3817,9 @@
       <c r="K201" s="11"/>
       <c r="L201" s="11"/>
       <c r="M201" s="13"/>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N201" s="13"/>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A202" s="11"/>
       <c r="B202" s="11"/>
       <c r="C202" s="11"/>
@@ -3632,8 +3833,9 @@
       <c r="K202" s="11"/>
       <c r="L202" s="11"/>
       <c r="M202" s="13"/>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N202" s="13"/>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A203" s="11"/>
       <c r="B203" s="11"/>
       <c r="C203" s="11"/>
@@ -3647,8 +3849,9 @@
       <c r="K203" s="11"/>
       <c r="L203" s="11"/>
       <c r="M203" s="13"/>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N203" s="13"/>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A204" s="11"/>
       <c r="B204" s="11"/>
       <c r="C204" s="11"/>
@@ -3662,8 +3865,9 @@
       <c r="K204" s="11"/>
       <c r="L204" s="11"/>
       <c r="M204" s="13"/>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N204" s="13"/>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A205" s="11"/>
       <c r="B205" s="11"/>
       <c r="C205" s="11"/>
@@ -3677,8 +3881,9 @@
       <c r="K205" s="11"/>
       <c r="L205" s="11"/>
       <c r="M205" s="13"/>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N205" s="13"/>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A206" s="11"/>
       <c r="B206" s="11"/>
       <c r="C206" s="11"/>
@@ -3692,8 +3897,9 @@
       <c r="K206" s="11"/>
       <c r="L206" s="11"/>
       <c r="M206" s="13"/>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N206" s="13"/>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A207" s="11"/>
       <c r="B207" s="11"/>
       <c r="C207" s="11"/>
@@ -3707,8 +3913,9 @@
       <c r="K207" s="11"/>
       <c r="L207" s="11"/>
       <c r="M207" s="13"/>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N207" s="13"/>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A208" s="11"/>
       <c r="B208" s="11"/>
       <c r="C208" s="11"/>
@@ -3722,8 +3929,9 @@
       <c r="K208" s="11"/>
       <c r="L208" s="11"/>
       <c r="M208" s="13"/>
-    </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N208" s="13"/>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A209" s="11"/>
       <c r="B209" s="11"/>
       <c r="C209" s="11"/>
@@ -3737,8 +3945,9 @@
       <c r="K209" s="11"/>
       <c r="L209" s="11"/>
       <c r="M209" s="13"/>
-    </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N209" s="13"/>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A210" s="11"/>
       <c r="B210" s="11"/>
       <c r="C210" s="11"/>
@@ -3752,8 +3961,9 @@
       <c r="K210" s="11"/>
       <c r="L210" s="11"/>
       <c r="M210" s="13"/>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N210" s="13"/>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A211" s="11"/>
       <c r="B211" s="11"/>
       <c r="C211" s="11"/>
@@ -3767,8 +3977,9 @@
       <c r="K211" s="11"/>
       <c r="L211" s="11"/>
       <c r="M211" s="13"/>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N211" s="13"/>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A212" s="11"/>
       <c r="B212" s="11"/>
       <c r="C212" s="11"/>
@@ -3782,8 +3993,9 @@
       <c r="K212" s="11"/>
       <c r="L212" s="11"/>
       <c r="M212" s="13"/>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N212" s="13"/>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A213" s="11"/>
       <c r="B213" s="11"/>
       <c r="C213" s="11"/>
@@ -3797,8 +4009,9 @@
       <c r="K213" s="11"/>
       <c r="L213" s="11"/>
       <c r="M213" s="13"/>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N213" s="13"/>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A214" s="11"/>
       <c r="B214" s="11"/>
       <c r="C214" s="11"/>
@@ -3812,8 +4025,9 @@
       <c r="K214" s="11"/>
       <c r="L214" s="11"/>
       <c r="M214" s="13"/>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N214" s="13"/>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A215" s="11"/>
       <c r="B215" s="11"/>
       <c r="C215" s="11"/>
@@ -3827,8 +4041,9 @@
       <c r="K215" s="11"/>
       <c r="L215" s="11"/>
       <c r="M215" s="13"/>
-    </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N215" s="13"/>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A216" s="11"/>
       <c r="B216" s="11"/>
       <c r="C216" s="11"/>
@@ -3842,8 +4057,9 @@
       <c r="K216" s="11"/>
       <c r="L216" s="11"/>
       <c r="M216" s="13"/>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N216" s="13"/>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A217" s="11"/>
       <c r="B217" s="11"/>
       <c r="C217" s="11"/>
@@ -3857,8 +4073,9 @@
       <c r="K217" s="11"/>
       <c r="L217" s="11"/>
       <c r="M217" s="13"/>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N217" s="13"/>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A218" s="11"/>
       <c r="B218" s="11"/>
       <c r="C218" s="11"/>
@@ -3872,8 +4089,9 @@
       <c r="K218" s="11"/>
       <c r="L218" s="11"/>
       <c r="M218" s="13"/>
-    </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N218" s="13"/>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A219" s="11"/>
       <c r="B219" s="11"/>
       <c r="C219" s="11"/>
@@ -3887,8 +4105,9 @@
       <c r="K219" s="11"/>
       <c r="L219" s="11"/>
       <c r="M219" s="13"/>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N219" s="13"/>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A220" s="11"/>
       <c r="B220" s="11"/>
       <c r="C220" s="11"/>
@@ -3902,8 +4121,9 @@
       <c r="K220" s="11"/>
       <c r="L220" s="11"/>
       <c r="M220" s="13"/>
-    </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N220" s="13"/>
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A221" s="11"/>
       <c r="B221" s="11"/>
       <c r="C221" s="11"/>
@@ -3917,8 +4137,9 @@
       <c r="K221" s="11"/>
       <c r="L221" s="11"/>
       <c r="M221" s="13"/>
-    </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N221" s="13"/>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A222" s="11"/>
       <c r="B222" s="11"/>
       <c r="C222" s="11"/>
@@ -3932,8 +4153,9 @@
       <c r="K222" s="11"/>
       <c r="L222" s="11"/>
       <c r="M222" s="13"/>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N222" s="13"/>
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A223" s="11"/>
       <c r="B223" s="11"/>
       <c r="C223" s="11"/>
@@ -3947,8 +4169,9 @@
       <c r="K223" s="11"/>
       <c r="L223" s="11"/>
       <c r="M223" s="13"/>
-    </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N223" s="13"/>
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A224" s="11"/>
       <c r="B224" s="11"/>
       <c r="C224" s="11"/>
@@ -3962,8 +4185,9 @@
       <c r="K224" s="11"/>
       <c r="L224" s="11"/>
       <c r="M224" s="13"/>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N224" s="13"/>
+    </row>
+    <row r="225" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A225" s="11"/>
       <c r="B225" s="11"/>
       <c r="C225" s="11"/>
@@ -3977,8 +4201,9 @@
       <c r="K225" s="11"/>
       <c r="L225" s="11"/>
       <c r="M225" s="13"/>
-    </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N225" s="13"/>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A226" s="11"/>
       <c r="B226" s="11"/>
       <c r="C226" s="11"/>
@@ -3992,8 +4217,9 @@
       <c r="K226" s="11"/>
       <c r="L226" s="11"/>
       <c r="M226" s="13"/>
-    </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N226" s="13"/>
+    </row>
+    <row r="227" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A227" s="11"/>
       <c r="B227" s="11"/>
       <c r="C227" s="11"/>
@@ -4007,8 +4233,9 @@
       <c r="K227" s="11"/>
       <c r="L227" s="11"/>
       <c r="M227" s="13"/>
-    </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N227" s="13"/>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A228" s="11"/>
       <c r="B228" s="11"/>
       <c r="C228" s="11"/>
@@ -4022,8 +4249,9 @@
       <c r="K228" s="11"/>
       <c r="L228" s="11"/>
       <c r="M228" s="13"/>
-    </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N228" s="13"/>
+    </row>
+    <row r="229" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A229" s="11"/>
       <c r="B229" s="11"/>
       <c r="C229" s="11"/>
@@ -4037,8 +4265,9 @@
       <c r="K229" s="11"/>
       <c r="L229" s="11"/>
       <c r="M229" s="13"/>
-    </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N229" s="13"/>
+    </row>
+    <row r="230" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A230" s="11"/>
       <c r="B230" s="11"/>
       <c r="C230" s="11"/>
@@ -4052,8 +4281,9 @@
       <c r="K230" s="11"/>
       <c r="L230" s="11"/>
       <c r="M230" s="13"/>
-    </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N230" s="13"/>
+    </row>
+    <row r="231" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A231" s="11"/>
       <c r="B231" s="11"/>
       <c r="C231" s="11"/>
@@ -4067,8 +4297,9 @@
       <c r="K231" s="11"/>
       <c r="L231" s="11"/>
       <c r="M231" s="13"/>
-    </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N231" s="13"/>
+    </row>
+    <row r="232" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A232" s="11"/>
       <c r="B232" s="11"/>
       <c r="C232" s="11"/>
@@ -4082,8 +4313,9 @@
       <c r="K232" s="11"/>
       <c r="L232" s="11"/>
       <c r="M232" s="13"/>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N232" s="13"/>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A233" s="11"/>
       <c r="B233" s="11"/>
       <c r="C233" s="11"/>
@@ -4097,8 +4329,9 @@
       <c r="K233" s="11"/>
       <c r="L233" s="11"/>
       <c r="M233" s="13"/>
-    </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N233" s="13"/>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A234" s="11"/>
       <c r="B234" s="11"/>
       <c r="C234" s="11"/>
@@ -4112,8 +4345,9 @@
       <c r="K234" s="11"/>
       <c r="L234" s="11"/>
       <c r="M234" s="13"/>
-    </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N234" s="13"/>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A235" s="11"/>
       <c r="B235" s="11"/>
       <c r="C235" s="11"/>
@@ -4127,8 +4361,9 @@
       <c r="K235" s="11"/>
       <c r="L235" s="11"/>
       <c r="M235" s="13"/>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N235" s="13"/>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A236" s="11"/>
       <c r="B236" s="11"/>
       <c r="C236" s="11"/>
@@ -4142,8 +4377,9 @@
       <c r="K236" s="11"/>
       <c r="L236" s="11"/>
       <c r="M236" s="13"/>
-    </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N236" s="13"/>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A237" s="11"/>
       <c r="B237" s="11"/>
       <c r="C237" s="11"/>
@@ -4157,8 +4393,9 @@
       <c r="K237" s="11"/>
       <c r="L237" s="11"/>
       <c r="M237" s="13"/>
-    </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N237" s="13"/>
+    </row>
+    <row r="238" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A238" s="11"/>
       <c r="B238" s="11"/>
       <c r="C238" s="11"/>
@@ -4172,8 +4409,9 @@
       <c r="K238" s="11"/>
       <c r="L238" s="11"/>
       <c r="M238" s="13"/>
-    </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N238" s="13"/>
+    </row>
+    <row r="239" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A239" s="11"/>
       <c r="B239" s="11"/>
       <c r="C239" s="11"/>
@@ -4187,8 +4425,9 @@
       <c r="K239" s="11"/>
       <c r="L239" s="11"/>
       <c r="M239" s="13"/>
-    </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N239" s="13"/>
+    </row>
+    <row r="240" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A240" s="11"/>
       <c r="B240" s="11"/>
       <c r="C240" s="11"/>
@@ -4202,8 +4441,9 @@
       <c r="K240" s="11"/>
       <c r="L240" s="11"/>
       <c r="M240" s="13"/>
-    </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N240" s="13"/>
+    </row>
+    <row r="241" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A241" s="11"/>
       <c r="B241" s="11"/>
       <c r="C241" s="11"/>
@@ -4217,8 +4457,9 @@
       <c r="K241" s="11"/>
       <c r="L241" s="11"/>
       <c r="M241" s="13"/>
-    </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N241" s="13"/>
+    </row>
+    <row r="242" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A242" s="11"/>
       <c r="B242" s="11"/>
       <c r="C242" s="11"/>
@@ -4232,8 +4473,9 @@
       <c r="K242" s="11"/>
       <c r="L242" s="11"/>
       <c r="M242" s="13"/>
-    </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N242" s="13"/>
+    </row>
+    <row r="243" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A243" s="11"/>
       <c r="B243" s="11"/>
       <c r="C243" s="11"/>
@@ -4247,8 +4489,9 @@
       <c r="K243" s="11"/>
       <c r="L243" s="11"/>
       <c r="M243" s="13"/>
-    </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N243" s="13"/>
+    </row>
+    <row r="244" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A244" s="11"/>
       <c r="B244" s="11"/>
       <c r="C244" s="11"/>
@@ -4262,8 +4505,9 @@
       <c r="K244" s="11"/>
       <c r="L244" s="11"/>
       <c r="M244" s="13"/>
-    </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N244" s="13"/>
+    </row>
+    <row r="245" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A245" s="11"/>
       <c r="B245" s="11"/>
       <c r="C245" s="11"/>
@@ -4277,8 +4521,9 @@
       <c r="K245" s="11"/>
       <c r="L245" s="11"/>
       <c r="M245" s="13"/>
-    </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N245" s="13"/>
+    </row>
+    <row r="246" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A246" s="11"/>
       <c r="B246" s="11"/>
       <c r="C246" s="11"/>
@@ -4292,8 +4537,9 @@
       <c r="K246" s="11"/>
       <c r="L246" s="11"/>
       <c r="M246" s="13"/>
-    </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N246" s="13"/>
+    </row>
+    <row r="247" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A247" s="11"/>
       <c r="B247" s="11"/>
       <c r="C247" s="11"/>
@@ -4307,8 +4553,9 @@
       <c r="K247" s="11"/>
       <c r="L247" s="11"/>
       <c r="M247" s="13"/>
-    </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N247" s="13"/>
+    </row>
+    <row r="248" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A248" s="11"/>
       <c r="B248" s="11"/>
       <c r="C248" s="11"/>
@@ -4322,8 +4569,9 @@
       <c r="K248" s="11"/>
       <c r="L248" s="11"/>
       <c r="M248" s="13"/>
-    </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N248" s="13"/>
+    </row>
+    <row r="249" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A249" s="11"/>
       <c r="B249" s="11"/>
       <c r="C249" s="11"/>
@@ -4337,8 +4585,9 @@
       <c r="K249" s="11"/>
       <c r="L249" s="11"/>
       <c r="M249" s="13"/>
-    </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N249" s="13"/>
+    </row>
+    <row r="250" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A250" s="11"/>
       <c r="B250" s="11"/>
       <c r="C250" s="11"/>
@@ -4352,8 +4601,9 @@
       <c r="K250" s="11"/>
       <c r="L250" s="11"/>
       <c r="M250" s="13"/>
-    </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N250" s="13"/>
+    </row>
+    <row r="251" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A251" s="11"/>
       <c r="B251" s="11"/>
       <c r="C251" s="11"/>
@@ -4367,8 +4617,9 @@
       <c r="K251" s="11"/>
       <c r="L251" s="11"/>
       <c r="M251" s="13"/>
-    </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N251" s="13"/>
+    </row>
+    <row r="252" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A252" s="11"/>
       <c r="B252" s="11"/>
       <c r="C252" s="11"/>
@@ -4382,8 +4633,9 @@
       <c r="K252" s="11"/>
       <c r="L252" s="11"/>
       <c r="M252" s="13"/>
-    </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N252" s="13"/>
+    </row>
+    <row r="253" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A253" s="11"/>
       <c r="B253" s="11"/>
       <c r="C253" s="11"/>
@@ -4397,8 +4649,9 @@
       <c r="K253" s="11"/>
       <c r="L253" s="11"/>
       <c r="M253" s="13"/>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N253" s="13"/>
+    </row>
+    <row r="254" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A254" s="11"/>
       <c r="B254" s="11"/>
       <c r="C254" s="11"/>
@@ -4412,8 +4665,9 @@
       <c r="K254" s="11"/>
       <c r="L254" s="11"/>
       <c r="M254" s="13"/>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N254" s="13"/>
+    </row>
+    <row r="255" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A255" s="11"/>
       <c r="B255" s="11"/>
       <c r="C255" s="11"/>
@@ -4427,8 +4681,9 @@
       <c r="K255" s="11"/>
       <c r="L255" s="11"/>
       <c r="M255" s="13"/>
-    </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N255" s="13"/>
+    </row>
+    <row r="256" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A256" s="11"/>
       <c r="B256" s="11"/>
       <c r="C256" s="11"/>
@@ -4442,8 +4697,9 @@
       <c r="K256" s="11"/>
       <c r="L256" s="11"/>
       <c r="M256" s="13"/>
-    </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N256" s="13"/>
+    </row>
+    <row r="257" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A257" s="11"/>
       <c r="B257" s="11"/>
       <c r="C257" s="11"/>
@@ -4457,8 +4713,9 @@
       <c r="K257" s="11"/>
       <c r="L257" s="11"/>
       <c r="M257" s="13"/>
-    </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N257" s="13"/>
+    </row>
+    <row r="258" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A258" s="11"/>
       <c r="B258" s="11"/>
       <c r="C258" s="11"/>
@@ -4472,8 +4729,9 @@
       <c r="K258" s="11"/>
       <c r="L258" s="11"/>
       <c r="M258" s="13"/>
-    </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N258" s="13"/>
+    </row>
+    <row r="259" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A259" s="11"/>
       <c r="B259" s="11"/>
       <c r="C259" s="11"/>
@@ -4487,8 +4745,9 @@
       <c r="K259" s="11"/>
       <c r="L259" s="11"/>
       <c r="M259" s="13"/>
-    </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N259" s="13"/>
+    </row>
+    <row r="260" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A260" s="11"/>
       <c r="B260" s="11"/>
       <c r="C260" s="11"/>
@@ -4502,8 +4761,9 @@
       <c r="K260" s="11"/>
       <c r="L260" s="11"/>
       <c r="M260" s="13"/>
-    </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N260" s="13"/>
+    </row>
+    <row r="261" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A261" s="11"/>
       <c r="B261" s="11"/>
       <c r="C261" s="11"/>
@@ -4517,8 +4777,9 @@
       <c r="K261" s="11"/>
       <c r="L261" s="11"/>
       <c r="M261" s="13"/>
-    </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N261" s="13"/>
+    </row>
+    <row r="262" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A262" s="11"/>
       <c r="B262" s="11"/>
       <c r="C262" s="11"/>
@@ -4532,8 +4793,9 @@
       <c r="K262" s="11"/>
       <c r="L262" s="11"/>
       <c r="M262" s="13"/>
-    </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N262" s="13"/>
+    </row>
+    <row r="263" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A263" s="11"/>
       <c r="B263" s="11"/>
       <c r="C263" s="11"/>
@@ -4547,8 +4809,9 @@
       <c r="K263" s="11"/>
       <c r="L263" s="11"/>
       <c r="M263" s="13"/>
-    </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N263" s="13"/>
+    </row>
+    <row r="264" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A264" s="11"/>
       <c r="B264" s="11"/>
       <c r="C264" s="11"/>
@@ -4562,8 +4825,9 @@
       <c r="K264" s="11"/>
       <c r="L264" s="11"/>
       <c r="M264" s="13"/>
-    </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N264" s="13"/>
+    </row>
+    <row r="265" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A265" s="11"/>
       <c r="B265" s="11"/>
       <c r="C265" s="11"/>
@@ -4577,8 +4841,9 @@
       <c r="K265" s="11"/>
       <c r="L265" s="11"/>
       <c r="M265" s="13"/>
-    </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N265" s="13"/>
+    </row>
+    <row r="266" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A266" s="11"/>
       <c r="B266" s="11"/>
       <c r="C266" s="11"/>
@@ -4592,8 +4857,9 @@
       <c r="K266" s="11"/>
       <c r="L266" s="11"/>
       <c r="M266" s="13"/>
-    </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N266" s="13"/>
+    </row>
+    <row r="267" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A267" s="11"/>
       <c r="B267" s="11"/>
       <c r="C267" s="11"/>
@@ -4607,8 +4873,9 @@
       <c r="K267" s="11"/>
       <c r="L267" s="11"/>
       <c r="M267" s="13"/>
-    </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N267" s="13"/>
+    </row>
+    <row r="268" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A268" s="11"/>
       <c r="B268" s="11"/>
       <c r="C268" s="11"/>
@@ -4622,8 +4889,9 @@
       <c r="K268" s="11"/>
       <c r="L268" s="11"/>
       <c r="M268" s="13"/>
-    </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N268" s="13"/>
+    </row>
+    <row r="269" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A269" s="11"/>
       <c r="B269" s="11"/>
       <c r="C269" s="11"/>
@@ -4637,8 +4905,9 @@
       <c r="K269" s="11"/>
       <c r="L269" s="11"/>
       <c r="M269" s="13"/>
-    </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N269" s="13"/>
+    </row>
+    <row r="270" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A270" s="11"/>
       <c r="B270" s="11"/>
       <c r="C270" s="11"/>
@@ -4652,8 +4921,9 @@
       <c r="K270" s="11"/>
       <c r="L270" s="11"/>
       <c r="M270" s="13"/>
-    </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N270" s="13"/>
+    </row>
+    <row r="271" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A271" s="11"/>
       <c r="B271" s="11"/>
       <c r="C271" s="11"/>
@@ -4667,8 +4937,9 @@
       <c r="K271" s="11"/>
       <c r="L271" s="11"/>
       <c r="M271" s="13"/>
-    </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N271" s="13"/>
+    </row>
+    <row r="272" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A272" s="11"/>
       <c r="B272" s="11"/>
       <c r="C272" s="11"/>
@@ -4682,8 +4953,9 @@
       <c r="K272" s="11"/>
       <c r="L272" s="11"/>
       <c r="M272" s="13"/>
-    </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N272" s="13"/>
+    </row>
+    <row r="273" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A273" s="11"/>
       <c r="B273" s="11"/>
       <c r="C273" s="11"/>
@@ -4697,8 +4969,9 @@
       <c r="K273" s="11"/>
       <c r="L273" s="11"/>
       <c r="M273" s="13"/>
-    </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N273" s="13"/>
+    </row>
+    <row r="274" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A274" s="11"/>
       <c r="B274" s="11"/>
       <c r="C274" s="11"/>
@@ -4712,8 +4985,9 @@
       <c r="K274" s="11"/>
       <c r="L274" s="11"/>
       <c r="M274" s="13"/>
-    </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N274" s="13"/>
+    </row>
+    <row r="275" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A275" s="11"/>
       <c r="B275" s="11"/>
       <c r="C275" s="11"/>
@@ -4727,8 +5001,9 @@
       <c r="K275" s="11"/>
       <c r="L275" s="11"/>
       <c r="M275" s="13"/>
-    </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N275" s="13"/>
+    </row>
+    <row r="276" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A276" s="11"/>
       <c r="B276" s="11"/>
       <c r="C276" s="11"/>
@@ -4742,8 +5017,9 @@
       <c r="K276" s="11"/>
       <c r="L276" s="11"/>
       <c r="M276" s="13"/>
-    </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N276" s="13"/>
+    </row>
+    <row r="277" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A277" s="11"/>
       <c r="B277" s="11"/>
       <c r="C277" s="11"/>
@@ -4757,8 +5033,9 @@
       <c r="K277" s="11"/>
       <c r="L277" s="11"/>
       <c r="M277" s="13"/>
-    </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N277" s="13"/>
+    </row>
+    <row r="278" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A278" s="11"/>
       <c r="B278" s="11"/>
       <c r="C278" s="11"/>
@@ -4772,8 +5049,9 @@
       <c r="K278" s="11"/>
       <c r="L278" s="11"/>
       <c r="M278" s="13"/>
-    </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N278" s="13"/>
+    </row>
+    <row r="279" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A279" s="11"/>
       <c r="B279" s="11"/>
       <c r="C279" s="11"/>
@@ -4787,8 +5065,9 @@
       <c r="K279" s="11"/>
       <c r="L279" s="11"/>
       <c r="M279" s="13"/>
-    </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N279" s="13"/>
+    </row>
+    <row r="280" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A280" s="11"/>
       <c r="B280" s="11"/>
       <c r="C280" s="11"/>
@@ -4802,8 +5081,9 @@
       <c r="K280" s="11"/>
       <c r="L280" s="11"/>
       <c r="M280" s="13"/>
-    </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N280" s="13"/>
+    </row>
+    <row r="281" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A281" s="11"/>
       <c r="B281" s="11"/>
       <c r="C281" s="11"/>
@@ -4817,8 +5097,9 @@
       <c r="K281" s="11"/>
       <c r="L281" s="11"/>
       <c r="M281" s="13"/>
-    </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N281" s="13"/>
+    </row>
+    <row r="282" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A282" s="11"/>
       <c r="B282" s="11"/>
       <c r="C282" s="11"/>
@@ -4832,8 +5113,9 @@
       <c r="K282" s="11"/>
       <c r="L282" s="11"/>
       <c r="M282" s="13"/>
-    </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N282" s="13"/>
+    </row>
+    <row r="283" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A283" s="11"/>
       <c r="B283" s="11"/>
       <c r="C283" s="11"/>
@@ -4847,8 +5129,9 @@
       <c r="K283" s="11"/>
       <c r="L283" s="11"/>
       <c r="M283" s="13"/>
-    </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N283" s="13"/>
+    </row>
+    <row r="284" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A284" s="11"/>
       <c r="B284" s="11"/>
       <c r="C284" s="11"/>
@@ -4862,8 +5145,9 @@
       <c r="K284" s="11"/>
       <c r="L284" s="11"/>
       <c r="M284" s="13"/>
-    </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N284" s="13"/>
+    </row>
+    <row r="285" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A285" s="11"/>
       <c r="B285" s="11"/>
       <c r="C285" s="11"/>
@@ -4877,8 +5161,9 @@
       <c r="K285" s="11"/>
       <c r="L285" s="11"/>
       <c r="M285" s="13"/>
-    </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N285" s="13"/>
+    </row>
+    <row r="286" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A286" s="11"/>
       <c r="B286" s="11"/>
       <c r="C286" s="11"/>
@@ -4892,8 +5177,9 @@
       <c r="K286" s="11"/>
       <c r="L286" s="11"/>
       <c r="M286" s="13"/>
-    </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N286" s="13"/>
+    </row>
+    <row r="287" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A287" s="11"/>
       <c r="B287" s="11"/>
       <c r="C287" s="11"/>
@@ -4907,8 +5193,9 @@
       <c r="K287" s="11"/>
       <c r="L287" s="11"/>
       <c r="M287" s="13"/>
-    </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N287" s="13"/>
+    </row>
+    <row r="288" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A288" s="11"/>
       <c r="B288" s="11"/>
       <c r="C288" s="11"/>
@@ -4922,8 +5209,9 @@
       <c r="K288" s="11"/>
       <c r="L288" s="11"/>
       <c r="M288" s="13"/>
-    </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N288" s="13"/>
+    </row>
+    <row r="289" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A289" s="11"/>
       <c r="B289" s="11"/>
       <c r="C289" s="11"/>
@@ -4937,8 +5225,9 @@
       <c r="K289" s="11"/>
       <c r="L289" s="11"/>
       <c r="M289" s="13"/>
-    </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N289" s="13"/>
+    </row>
+    <row r="290" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A290" s="11"/>
       <c r="B290" s="11"/>
       <c r="C290" s="11"/>
@@ -4952,8 +5241,9 @@
       <c r="K290" s="11"/>
       <c r="L290" s="11"/>
       <c r="M290" s="13"/>
-    </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N290" s="13"/>
+    </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A291" s="11"/>
       <c r="B291" s="11"/>
       <c r="C291" s="11"/>
@@ -4967,8 +5257,9 @@
       <c r="K291" s="11"/>
       <c r="L291" s="11"/>
       <c r="M291" s="13"/>
-    </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N291" s="13"/>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A292" s="11"/>
       <c r="B292" s="11"/>
       <c r="C292" s="11"/>
@@ -4982,8 +5273,9 @@
       <c r="K292" s="11"/>
       <c r="L292" s="11"/>
       <c r="M292" s="13"/>
-    </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N292" s="13"/>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A293" s="11"/>
       <c r="B293" s="11"/>
       <c r="C293" s="11"/>
@@ -4997,8 +5289,9 @@
       <c r="K293" s="11"/>
       <c r="L293" s="11"/>
       <c r="M293" s="13"/>
-    </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N293" s="13"/>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A294" s="11"/>
       <c r="B294" s="11"/>
       <c r="C294" s="11"/>
@@ -5012,8 +5305,9 @@
       <c r="K294" s="11"/>
       <c r="L294" s="11"/>
       <c r="M294" s="13"/>
-    </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N294" s="13"/>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A295" s="11"/>
       <c r="B295" s="11"/>
       <c r="C295" s="11"/>
@@ -5027,8 +5321,9 @@
       <c r="K295" s="11"/>
       <c r="L295" s="11"/>
       <c r="M295" s="13"/>
-    </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N295" s="13"/>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A296" s="11"/>
       <c r="B296" s="11"/>
       <c r="C296" s="11"/>
@@ -5042,8 +5337,9 @@
       <c r="K296" s="11"/>
       <c r="L296" s="11"/>
       <c r="M296" s="13"/>
-    </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N296" s="13"/>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A297" s="11"/>
       <c r="B297" s="11"/>
       <c r="C297" s="11"/>
@@ -5057,8 +5353,9 @@
       <c r="K297" s="11"/>
       <c r="L297" s="11"/>
       <c r="M297" s="13"/>
-    </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N297" s="13"/>
+    </row>
+    <row r="298" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A298" s="11"/>
       <c r="B298" s="11"/>
       <c r="C298" s="11"/>
@@ -5072,8 +5369,9 @@
       <c r="K298" s="11"/>
       <c r="L298" s="11"/>
       <c r="M298" s="13"/>
-    </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N298" s="13"/>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A299" s="11"/>
       <c r="B299" s="11"/>
       <c r="C299" s="11"/>
@@ -5087,8 +5385,9 @@
       <c r="K299" s="11"/>
       <c r="L299" s="11"/>
       <c r="M299" s="13"/>
-    </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N299" s="13"/>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A300" s="11"/>
       <c r="B300" s="11"/>
       <c r="C300" s="11"/>
@@ -5102,8 +5401,9 @@
       <c r="K300" s="11"/>
       <c r="L300" s="11"/>
       <c r="M300" s="13"/>
-    </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N300" s="13"/>
+    </row>
+    <row r="301" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A301" s="11"/>
       <c r="B301" s="11"/>
       <c r="C301" s="11"/>
@@ -5117,8 +5417,9 @@
       <c r="K301" s="11"/>
       <c r="L301" s="11"/>
       <c r="M301" s="13"/>
-    </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N301" s="13"/>
+    </row>
+    <row r="302" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A302" s="11"/>
       <c r="B302" s="11"/>
       <c r="C302" s="11"/>
@@ -5132,8 +5433,9 @@
       <c r="K302" s="11"/>
       <c r="L302" s="11"/>
       <c r="M302" s="13"/>
-    </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N302" s="13"/>
+    </row>
+    <row r="303" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A303" s="11"/>
       <c r="B303" s="11"/>
       <c r="C303" s="11"/>
@@ -5147,8 +5449,9 @@
       <c r="K303" s="11"/>
       <c r="L303" s="11"/>
       <c r="M303" s="13"/>
-    </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N303" s="13"/>
+    </row>
+    <row r="304" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A304" s="11"/>
       <c r="B304" s="11"/>
       <c r="C304" s="11"/>
@@ -5162,8 +5465,9 @@
       <c r="K304" s="11"/>
       <c r="L304" s="11"/>
       <c r="M304" s="13"/>
-    </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N304" s="13"/>
+    </row>
+    <row r="305" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A305" s="11"/>
       <c r="B305" s="11"/>
       <c r="C305" s="11"/>
@@ -5177,8 +5481,9 @@
       <c r="K305" s="11"/>
       <c r="L305" s="11"/>
       <c r="M305" s="13"/>
-    </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N305" s="13"/>
+    </row>
+    <row r="306" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A306" s="11"/>
       <c r="B306" s="11"/>
       <c r="C306" s="11"/>
@@ -5192,8 +5497,9 @@
       <c r="K306" s="11"/>
       <c r="L306" s="11"/>
       <c r="M306" s="13"/>
-    </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N306" s="13"/>
+    </row>
+    <row r="307" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A307" s="11"/>
       <c r="B307" s="11"/>
       <c r="C307" s="11"/>
@@ -5207,8 +5513,9 @@
       <c r="K307" s="11"/>
       <c r="L307" s="11"/>
       <c r="M307" s="13"/>
-    </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N307" s="13"/>
+    </row>
+    <row r="308" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A308" s="11"/>
       <c r="B308" s="11"/>
       <c r="C308" s="11"/>
@@ -5222,8 +5529,9 @@
       <c r="K308" s="11"/>
       <c r="L308" s="11"/>
       <c r="M308" s="13"/>
-    </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N308" s="13"/>
+    </row>
+    <row r="309" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A309" s="11"/>
       <c r="B309" s="11"/>
       <c r="C309" s="11"/>
@@ -5237,8 +5545,9 @@
       <c r="K309" s="11"/>
       <c r="L309" s="11"/>
       <c r="M309" s="13"/>
-    </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N309" s="13"/>
+    </row>
+    <row r="310" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A310" s="11"/>
       <c r="B310" s="11"/>
       <c r="C310" s="11"/>
@@ -5252,8 +5561,9 @@
       <c r="K310" s="11"/>
       <c r="L310" s="11"/>
       <c r="M310" s="13"/>
-    </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N310" s="13"/>
+    </row>
+    <row r="311" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A311" s="11"/>
       <c r="B311" s="11"/>
       <c r="C311" s="11"/>
@@ -5267,8 +5577,9 @@
       <c r="K311" s="11"/>
       <c r="L311" s="11"/>
       <c r="M311" s="13"/>
-    </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N311" s="13"/>
+    </row>
+    <row r="312" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A312" s="11"/>
       <c r="B312" s="11"/>
       <c r="C312" s="11"/>
@@ -5282,8 +5593,9 @@
       <c r="K312" s="11"/>
       <c r="L312" s="11"/>
       <c r="M312" s="13"/>
-    </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N312" s="13"/>
+    </row>
+    <row r="313" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A313" s="11"/>
       <c r="B313" s="11"/>
       <c r="C313" s="11"/>
@@ -5297,8 +5609,9 @@
       <c r="K313" s="11"/>
       <c r="L313" s="11"/>
       <c r="M313" s="13"/>
-    </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N313" s="13"/>
+    </row>
+    <row r="314" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A314" s="11"/>
       <c r="B314" s="11"/>
       <c r="C314" s="11"/>
@@ -5312,8 +5625,9 @@
       <c r="K314" s="11"/>
       <c r="L314" s="11"/>
       <c r="M314" s="13"/>
-    </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N314" s="13"/>
+    </row>
+    <row r="315" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A315" s="11"/>
       <c r="B315" s="11"/>
       <c r="C315" s="11"/>
@@ -5327,8 +5641,9 @@
       <c r="K315" s="11"/>
       <c r="L315" s="11"/>
       <c r="M315" s="13"/>
-    </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N315" s="13"/>
+    </row>
+    <row r="316" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A316" s="11"/>
       <c r="B316" s="11"/>
       <c r="C316" s="11"/>
@@ -5342,8 +5657,9 @@
       <c r="K316" s="11"/>
       <c r="L316" s="11"/>
       <c r="M316" s="13"/>
-    </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N316" s="13"/>
+    </row>
+    <row r="317" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A317" s="11"/>
       <c r="B317" s="11"/>
       <c r="C317" s="11"/>
@@ -5357,8 +5673,9 @@
       <c r="K317" s="11"/>
       <c r="L317" s="11"/>
       <c r="M317" s="13"/>
-    </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N317" s="13"/>
+    </row>
+    <row r="318" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A318" s="11"/>
       <c r="B318" s="11"/>
       <c r="C318" s="11"/>
@@ -5372,8 +5689,9 @@
       <c r="K318" s="11"/>
       <c r="L318" s="11"/>
       <c r="M318" s="13"/>
-    </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N318" s="13"/>
+    </row>
+    <row r="319" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A319" s="11"/>
       <c r="B319" s="11"/>
       <c r="C319" s="11"/>
@@ -5387,8 +5705,9 @@
       <c r="K319" s="11"/>
       <c r="L319" s="11"/>
       <c r="M319" s="13"/>
-    </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N319" s="13"/>
+    </row>
+    <row r="320" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A320" s="11"/>
       <c r="B320" s="11"/>
       <c r="C320" s="11"/>
@@ -5402,8 +5721,9 @@
       <c r="K320" s="11"/>
       <c r="L320" s="11"/>
       <c r="M320" s="13"/>
-    </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N320" s="13"/>
+    </row>
+    <row r="321" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A321" s="11"/>
       <c r="B321" s="11"/>
       <c r="C321" s="11"/>
@@ -5417,8 +5737,9 @@
       <c r="K321" s="11"/>
       <c r="L321" s="11"/>
       <c r="M321" s="13"/>
-    </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N321" s="13"/>
+    </row>
+    <row r="322" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A322" s="11"/>
       <c r="B322" s="11"/>
       <c r="C322" s="11"/>
@@ -5432,8 +5753,9 @@
       <c r="K322" s="11"/>
       <c r="L322" s="11"/>
       <c r="M322" s="13"/>
-    </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N322" s="13"/>
+    </row>
+    <row r="323" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A323" s="11"/>
       <c r="B323" s="11"/>
       <c r="C323" s="11"/>
@@ -5447,6 +5769,55 @@
       <c r="K323" s="11"/>
       <c r="L323" s="11"/>
       <c r="M323" s="13"/>
+      <c r="N323" s="13"/>
+    </row>
+    <row r="324" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A324" s="11"/>
+      <c r="B324" s="11"/>
+      <c r="C324" s="11"/>
+      <c r="D324" s="11"/>
+      <c r="E324" s="12"/>
+      <c r="F324" s="11"/>
+      <c r="G324" s="11"/>
+      <c r="H324" s="11"/>
+      <c r="I324" s="11"/>
+      <c r="J324" s="11"/>
+      <c r="K324" s="11"/>
+      <c r="L324" s="11"/>
+      <c r="M324" s="13"/>
+      <c r="N324" s="13"/>
+    </row>
+    <row r="325" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A325" s="11"/>
+      <c r="B325" s="11"/>
+      <c r="C325" s="11"/>
+      <c r="D325" s="11"/>
+      <c r="E325" s="12"/>
+      <c r="F325" s="11"/>
+      <c r="G325" s="11"/>
+      <c r="H325" s="11"/>
+      <c r="I325" s="11"/>
+      <c r="J325" s="11"/>
+      <c r="K325" s="11"/>
+      <c r="L325" s="11"/>
+      <c r="M325" s="13"/>
+      <c r="N325" s="13"/>
+    </row>
+    <row r="326" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A326" s="11"/>
+      <c r="B326" s="11"/>
+      <c r="C326" s="11"/>
+      <c r="D326" s="11"/>
+      <c r="E326" s="12"/>
+      <c r="F326" s="11"/>
+      <c r="G326" s="11"/>
+      <c r="H326" s="11"/>
+      <c r="I326" s="11"/>
+      <c r="J326" s="11"/>
+      <c r="K326" s="11"/>
+      <c r="L326" s="11"/>
+      <c r="M326" s="13"/>
+      <c r="N326" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>